<commit_message>
Actualización automática desde interfaz
</commit_message>
<xml_diff>
--- a/sensores.xlsx
+++ b/sensores.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1683"/>
+  <dimension ref="A1:F1709"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37457,6 +37457,578 @@
         <v>61.8</v>
       </c>
     </row>
+    <row r="1684">
+      <c r="A1684" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:24</t>
+        </is>
+      </c>
+      <c r="B1684" t="n">
+        <v>515</v>
+      </c>
+      <c r="C1684" t="n">
+        <v>21.02</v>
+      </c>
+      <c r="D1684" t="n">
+        <v>115.92</v>
+      </c>
+      <c r="E1684" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1684" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1685">
+      <c r="A1685" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:25</t>
+        </is>
+      </c>
+      <c r="B1685" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1685" t="n">
+        <v>21.02</v>
+      </c>
+      <c r="D1685" t="n">
+        <v>115.87</v>
+      </c>
+      <c r="E1685" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1685" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1686">
+      <c r="A1686" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:26</t>
+        </is>
+      </c>
+      <c r="B1686" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1686" t="n">
+        <v>21.02</v>
+      </c>
+      <c r="D1686" t="n">
+        <v>115.75</v>
+      </c>
+      <c r="E1686" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1686" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1687">
+      <c r="A1687" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:27</t>
+        </is>
+      </c>
+      <c r="B1687" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1687" t="n">
+        <v>20.53</v>
+      </c>
+      <c r="D1687" t="n">
+        <v>115.75</v>
+      </c>
+      <c r="E1687" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1687" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1688">
+      <c r="A1688" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:29</t>
+        </is>
+      </c>
+      <c r="B1688" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1688" t="n">
+        <v>20.53</v>
+      </c>
+      <c r="D1688" t="n">
+        <v>115.84</v>
+      </c>
+      <c r="E1688" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1688" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1689">
+      <c r="A1689" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:30</t>
+        </is>
+      </c>
+      <c r="B1689" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1689" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1689" t="n">
+        <v>115.77</v>
+      </c>
+      <c r="E1689" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1689" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1690">
+      <c r="A1690" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:31</t>
+        </is>
+      </c>
+      <c r="B1690" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1690" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1690" t="n">
+        <v>69.63</v>
+      </c>
+      <c r="E1690" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1690" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1691">
+      <c r="A1691" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:37</t>
+        </is>
+      </c>
+      <c r="B1691" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1691" t="n">
+        <v>21.02</v>
+      </c>
+      <c r="D1691" t="n">
+        <v>70.52</v>
+      </c>
+      <c r="E1691" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1691" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1692">
+      <c r="A1692" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:43</t>
+        </is>
+      </c>
+      <c r="B1692" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1692" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1692" t="n">
+        <v>70.52</v>
+      </c>
+      <c r="E1692" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1692" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1693">
+      <c r="A1693" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:44</t>
+        </is>
+      </c>
+      <c r="B1693" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1693" t="n">
+        <v>21.02</v>
+      </c>
+      <c r="D1693" t="n">
+        <v>69.7</v>
+      </c>
+      <c r="E1693" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1693" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1694">
+      <c r="A1694" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:45</t>
+        </is>
+      </c>
+      <c r="B1694" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1694" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1694" t="n">
+        <v>69.27</v>
+      </c>
+      <c r="E1694" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1694" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1695">
+      <c r="A1695" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:46</t>
+        </is>
+      </c>
+      <c r="B1695" t="n">
+        <v>515</v>
+      </c>
+      <c r="C1695" t="n">
+        <v>21.02</v>
+      </c>
+      <c r="D1695" t="n">
+        <v>69.7</v>
+      </c>
+      <c r="E1695" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1695" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1696">
+      <c r="A1696" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:47</t>
+        </is>
+      </c>
+      <c r="B1696" t="n">
+        <v>515</v>
+      </c>
+      <c r="C1696" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1696" t="n">
+        <v>69.72</v>
+      </c>
+      <c r="E1696" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1696" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1697">
+      <c r="A1697" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:48</t>
+        </is>
+      </c>
+      <c r="B1697" t="n">
+        <v>515</v>
+      </c>
+      <c r="C1697" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1697" t="n">
+        <v>70.52</v>
+      </c>
+      <c r="E1697" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1697" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1698">
+      <c r="A1698" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:49</t>
+        </is>
+      </c>
+      <c r="B1698" t="n">
+        <v>515</v>
+      </c>
+      <c r="C1698" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1698" t="n">
+        <v>70.06999999999999</v>
+      </c>
+      <c r="E1698" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1698" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1699">
+      <c r="A1699" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:50</t>
+        </is>
+      </c>
+      <c r="B1699" t="n">
+        <v>515</v>
+      </c>
+      <c r="C1699" t="n">
+        <v>21.02</v>
+      </c>
+      <c r="D1699" t="n">
+        <v>70.06</v>
+      </c>
+      <c r="E1699" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1699" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1700">
+      <c r="A1700" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:52</t>
+        </is>
+      </c>
+      <c r="B1700" t="n">
+        <v>515</v>
+      </c>
+      <c r="C1700" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1700" t="n">
+        <v>69.7</v>
+      </c>
+      <c r="E1700" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="F1700" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1701">
+      <c r="A1701" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:53</t>
+        </is>
+      </c>
+      <c r="B1701" t="n">
+        <v>515</v>
+      </c>
+      <c r="C1701" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1701" t="n">
+        <v>69.26000000000001</v>
+      </c>
+      <c r="E1701" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="F1701" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="1702">
+      <c r="A1702" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:54</t>
+        </is>
+      </c>
+      <c r="B1702" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1702" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="D1702" t="n">
+        <v>69.63</v>
+      </c>
+      <c r="E1702" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1702" t="n">
+        <v>67.59999999999999</v>
+      </c>
+    </row>
+    <row r="1703">
+      <c r="A1703" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:55</t>
+        </is>
+      </c>
+      <c r="B1703" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1703" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1703" t="n">
+        <v>69.63</v>
+      </c>
+      <c r="E1703" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1703" t="n">
+        <v>67.59999999999999</v>
+      </c>
+    </row>
+    <row r="1704">
+      <c r="A1704" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:56</t>
+        </is>
+      </c>
+      <c r="B1704" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1704" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1704" t="n">
+        <v>68.83</v>
+      </c>
+      <c r="E1704" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1704" t="n">
+        <v>67.59999999999999</v>
+      </c>
+    </row>
+    <row r="1705">
+      <c r="A1705" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:57</t>
+        </is>
+      </c>
+      <c r="B1705" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1705" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1705" t="n">
+        <v>69.27</v>
+      </c>
+      <c r="E1705" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F1705" t="n">
+        <v>67.59999999999999</v>
+      </c>
+    </row>
+    <row r="1706">
+      <c r="A1706" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:58</t>
+        </is>
+      </c>
+      <c r="B1706" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1706" t="n">
+        <v>20.53</v>
+      </c>
+      <c r="D1706" t="n">
+        <v>69.27</v>
+      </c>
+      <c r="E1706" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="F1706" t="n">
+        <v>67.59999999999999</v>
+      </c>
+    </row>
+    <row r="1707">
+      <c r="A1707" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:19:59</t>
+        </is>
+      </c>
+      <c r="B1707" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1707" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="D1707" t="n">
+        <v>68.83</v>
+      </c>
+      <c r="E1707" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="F1707" t="n">
+        <v>67.59999999999999</v>
+      </c>
+    </row>
+    <row r="1708">
+      <c r="A1708" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:20:00</t>
+        </is>
+      </c>
+      <c r="B1708" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1708" t="n">
+        <v>20.53</v>
+      </c>
+      <c r="D1708" t="n">
+        <v>69.27</v>
+      </c>
+      <c r="E1708" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="F1708" t="n">
+        <v>67.59999999999999</v>
+      </c>
+    </row>
+    <row r="1709">
+      <c r="A1709" t="inlineStr">
+        <is>
+          <t>2025-06-09 00:20:01</t>
+        </is>
+      </c>
+      <c r="B1709" t="n">
+        <v>516</v>
+      </c>
+      <c r="C1709" t="n">
+        <v>21.02</v>
+      </c>
+      <c r="D1709" t="n">
+        <v>68.83</v>
+      </c>
+      <c r="E1709" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="F1709" t="n">
+        <v>67.59999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>